<commit_message>
Update dashboard with latest changes and improvements - Jan 9 2026
</commit_message>
<xml_diff>
--- a/demodata/ZRFI005.XLSX
+++ b/demodata/ZRFI005.XLSX
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$102</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="273">
   <si>
     <t>1000</t>
   </si>
@@ -399,6 +399,18 @@
     <t>CÔNG TY TNHH THƯƠNG MẠI - XÂY DỰNG THIÊN HÀ PHÁT</t>
   </si>
   <si>
+    <t>10110766</t>
+  </si>
+  <si>
+    <t>PHẠM MINH SĨ</t>
+  </si>
+  <si>
+    <t>1200000854</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH TRẦN LIÊN HƯNG</t>
+  </si>
+  <si>
     <t>10810584</t>
   </si>
   <si>
@@ -486,18 +498,18 @@
     <t>CÔNG TY CỔ PHẦN ĐÔNG NGÔ MANUFACTURER</t>
   </si>
   <si>
+    <t>1200001029</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH TRANG TRÍ NỘI THẤT PHONG THẢO</t>
+  </si>
+  <si>
     <t>10400773</t>
   </si>
   <si>
     <t>VŨ ANH HAI</t>
   </si>
   <si>
-    <t>1200001029</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH TRANG TRÍ NỘI THẤT PHONG THẢO</t>
-  </si>
-  <si>
     <t>1200001030</t>
   </si>
   <si>
@@ -567,12 +579,6 @@
     <t>CÔNG TY TNHH SX TM QUANG TRUNG NGUYÊN</t>
   </si>
   <si>
-    <t>10110766</t>
-  </si>
-  <si>
-    <t>PHẠM MINH SĨ</t>
-  </si>
-  <si>
     <t>1200001079</t>
   </si>
   <si>
@@ -597,6 +603,12 @@
     <t>CÔNG TY TNHH TM SẢN XUẤT XNK NỘI THẤT MCS</t>
   </si>
   <si>
+    <t>1200001104</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN ARTEX ĐỒNG THÁP</t>
+  </si>
+  <si>
     <t>1200001109</t>
   </si>
   <si>
@@ -624,7 +636,7 @@
     <t>1200001118</t>
   </si>
   <si>
-    <t>Hoàng Sỹ Tiến</t>
+    <t>Pham Van Vuong</t>
   </si>
   <si>
     <t>1200001119</t>
@@ -663,57 +675,51 @@
     <t>VÕ CÔNG QUANG</t>
   </si>
   <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>1300000016</t>
+  </si>
+  <si>
+    <t>QUALITY IMAGE SDN BHD</t>
+  </si>
+  <si>
+    <t>1200000856</t>
+  </si>
+  <si>
+    <t>CÔNG TY TRÁCH NHIỆM HỮU HẠN AN PHÚ</t>
+  </si>
+  <si>
+    <t>1200000974</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH CAO VÕ</t>
+  </si>
+  <si>
+    <t>1200001004</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH MỘT THÀNH VIÊN XÂY DỰNG - THƯƠNG MẠI VÀ DỊCH VỤ HOÀNG GIA</t>
+  </si>
+  <si>
+    <t>1200000460</t>
+  </si>
+  <si>
+    <t>LÊ HỒNG TRƯỜNG</t>
+  </si>
+  <si>
+    <t>1200000820</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH SẢN XUẤT NỘI THẤT TRẦN TIẾN</t>
+  </si>
+  <si>
     <t>1200001144</t>
   </si>
   <si>
     <t>HỘ KINH DOANH BUÔN LÊ COFFEE</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>1300000016</t>
-  </si>
-  <si>
-    <t>QUALITY IMAGE SDN BHD</t>
-  </si>
-  <si>
-    <t>1200000854</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH TRẦN LIÊN HƯNG</t>
-  </si>
-  <si>
-    <t>1200000856</t>
-  </si>
-  <si>
-    <t>CÔNG TY TRÁCH NHIỆM HỮU HẠN AN PHÚ</t>
-  </si>
-  <si>
-    <t>1200000974</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH CAO VÕ</t>
-  </si>
-  <si>
-    <t>1200001004</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH MỘT THÀNH VIÊN XÂY DỰNG - THƯƠNG MẠI VÀ DỊCH VỤ HOÀNG GIA</t>
-  </si>
-  <si>
-    <t>1200000460</t>
-  </si>
-  <si>
-    <t>LÊ HỒNG TRƯỜNG</t>
-  </si>
-  <si>
-    <t>1200000820</t>
-  </si>
-  <si>
-    <t>CÔNG TY TNHH SẢN XUẤT NỘI THẤT TRẦN TIẾN</t>
-  </si>
-  <si>
     <t>1200000959</t>
   </si>
   <si>
@@ -748,6 +754,18 @@
   </si>
   <si>
     <t>CÔNG TY TNHH XÂY DỰNG VÀ THƯƠNG MẠI AN PHỤNG</t>
+  </si>
+  <si>
+    <t>1200001059</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN XÂY DỰNG - THƯƠNG MẠI - NỘI THẤT HH</t>
+  </si>
+  <si>
+    <t>1200001136</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH NỘI THẤT TÂM CASA</t>
   </si>
   <si>
     <t>Company Code</t>
@@ -1169,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y99"/>
+  <dimension ref="A1:Y102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1197,86 +1215,85 @@
     <col min="19" max="20" width="11" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -1415,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="2">
-        <v>0</v>
+        <v>361088859</v>
       </c>
       <c r="U3" s="2">
         <v>0</v>
@@ -1430,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="Y3" s="2">
-        <v>0</v>
+        <v>361088859</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1723,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>0</v>
+        <v>106074058</v>
       </c>
       <c r="U7" s="2">
         <v>0</v>
@@ -1738,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="2">
-        <v>0</v>
+        <v>106074058</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -2416,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="2">
-        <v>0</v>
+        <v>195415200</v>
       </c>
       <c r="U16" s="2">
         <v>0</v>
@@ -2431,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="Y16" s="2">
-        <v>0</v>
+        <v>195415200</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -3621,7 +3638,7 @@
         <v>9</v>
       </c>
       <c r="K32" s="2">
-        <v>45297965</v>
+        <v>70892323</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
@@ -3639,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="2">
-        <v>45297965</v>
+        <v>70892323</v>
       </c>
       <c r="R32" s="2">
         <v>0</v>
@@ -3722,10 +3739,10 @@
         <v>0</v>
       </c>
       <c r="S33" s="2">
-        <v>0</v>
+        <v>6787145</v>
       </c>
       <c r="T33" s="2">
-        <v>0</v>
+        <v>43212855</v>
       </c>
       <c r="U33" s="2">
         <v>0</v>
@@ -3740,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="Y33" s="2">
-        <v>0</v>
+        <v>50000000</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -4527,7 +4544,7 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="F44" t="s">
         <v>125</v>
@@ -4545,25 +4562,25 @@
         <v>9</v>
       </c>
       <c r="K44" s="2">
-        <v>8862904</v>
+        <v>0</v>
       </c>
       <c r="L44" s="2">
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <v>-458131</v>
+        <v>0</v>
       </c>
       <c r="N44" s="2">
         <v>0</v>
       </c>
       <c r="O44" s="2">
-        <v>0</v>
+        <v>-437763</v>
       </c>
       <c r="P44" s="2">
-        <v>0</v>
+        <v>-563094</v>
       </c>
       <c r="Q44" s="2">
-        <v>8404773</v>
+        <v>-1000857</v>
       </c>
       <c r="R44" s="2">
         <v>0</v>
@@ -4604,31 +4621,31 @@
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F45" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="G45" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="H45" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I45" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J45" t="s">
         <v>9</v>
       </c>
       <c r="K45" s="2">
-        <v>0</v>
+        <v>8862904</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
       </c>
       <c r="M45" s="2">
-        <v>0</v>
+        <v>-458131</v>
       </c>
       <c r="N45" s="2">
         <v>0</v>
@@ -4637,10 +4654,10 @@
         <v>0</v>
       </c>
       <c r="P45" s="2">
-        <v>25628426</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="2">
-        <v>25628426</v>
+        <v>8404773</v>
       </c>
       <c r="R45" s="2">
         <v>0</v>
@@ -4684,16 +4701,16 @@
         <v>118</v>
       </c>
       <c r="F46" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="G46" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="H46" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I46" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J46" t="s">
         <v>9</v>
@@ -4705,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="2">
-        <v>-840131</v>
+        <v>0</v>
       </c>
       <c r="N46" s="2">
         <v>0</v>
@@ -4714,10 +4731,10 @@
         <v>0</v>
       </c>
       <c r="P46" s="2">
-        <v>0</v>
+        <v>25628426</v>
       </c>
       <c r="Q46" s="2">
-        <v>-840131</v>
+        <v>25628426</v>
       </c>
       <c r="R46" s="2">
         <v>0</v>
@@ -4758,43 +4775,43 @@
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="F47" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G47" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H47" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I47" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J47" t="s">
         <v>9</v>
       </c>
       <c r="K47" s="2">
-        <v>8553717</v>
+        <v>0</v>
       </c>
       <c r="L47" s="2">
-        <v>38598624</v>
+        <v>0</v>
       </c>
       <c r="M47" s="2">
-        <v>0</v>
+        <v>-840131</v>
       </c>
       <c r="N47" s="2">
-        <v>5064037</v>
+        <v>0</v>
       </c>
       <c r="O47" s="2">
-        <v>42755331</v>
+        <v>0</v>
       </c>
       <c r="P47" s="2">
         <v>0</v>
       </c>
       <c r="Q47" s="2">
-        <v>94971709</v>
+        <v>-840131</v>
       </c>
       <c r="R47" s="2">
         <v>0</v>
@@ -4835,43 +4852,43 @@
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F48" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="G48" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="H48" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I48" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J48" t="s">
         <v>9</v>
       </c>
       <c r="K48" s="2">
-        <v>23064694</v>
+        <v>8553717</v>
       </c>
       <c r="L48" s="2">
-        <v>0</v>
+        <v>38598624</v>
       </c>
       <c r="M48" s="2">
         <v>0</v>
       </c>
       <c r="N48" s="2">
-        <v>0</v>
+        <v>5064037</v>
       </c>
       <c r="O48" s="2">
-        <v>0</v>
+        <v>42755331</v>
       </c>
       <c r="P48" s="2">
         <v>0</v>
       </c>
       <c r="Q48" s="2">
-        <v>23064694</v>
+        <v>94971709</v>
       </c>
       <c r="R48" s="2">
         <v>0</v>
@@ -4906,31 +4923,31 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="F49" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="G49" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="H49" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I49" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J49" t="s">
         <v>9</v>
       </c>
       <c r="K49" s="2">
-        <v>54874800</v>
+        <v>23064694</v>
       </c>
       <c r="L49" s="2">
         <v>0</v>
@@ -4948,7 +4965,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="2">
-        <v>54874800</v>
+        <v>23064694</v>
       </c>
       <c r="R49" s="2">
         <v>0</v>
@@ -4983,34 +5000,34 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="G50" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="H50" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I50" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J50" t="s">
         <v>9</v>
       </c>
       <c r="K50" s="2">
-        <v>304812288</v>
+        <v>54874800</v>
       </c>
       <c r="L50" s="2">
-        <v>143665920</v>
+        <v>0</v>
       </c>
       <c r="M50" s="2">
         <v>0</v>
@@ -5025,7 +5042,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="2">
-        <v>448478208</v>
+        <v>54874800</v>
       </c>
       <c r="R50" s="2">
         <v>0</v>
@@ -5060,34 +5077,34 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>106</v>
+        <v>19</v>
       </c>
       <c r="G51" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I51" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J51" t="s">
         <v>9</v>
       </c>
       <c r="K51" s="2">
-        <v>31110202</v>
+        <v>304812288</v>
       </c>
       <c r="L51" s="2">
-        <v>0</v>
+        <v>143665920</v>
       </c>
       <c r="M51" s="2">
         <v>0</v>
@@ -5102,7 +5119,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="2">
-        <v>31110202</v>
+        <v>448478208</v>
       </c>
       <c r="R51" s="2">
         <v>0</v>
@@ -5146,22 +5163,22 @@
         <v>96</v>
       </c>
       <c r="F52" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G52" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="H52" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I52" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J52" t="s">
         <v>9</v>
       </c>
       <c r="K52" s="2">
-        <v>3880646</v>
+        <v>31110202</v>
       </c>
       <c r="L52" s="2">
         <v>0</v>
@@ -5179,7 +5196,7 @@
         <v>0</v>
       </c>
       <c r="Q52" s="2">
-        <v>3880646</v>
+        <v>31110202</v>
       </c>
       <c r="R52" s="2">
         <v>0</v>
@@ -5214,31 +5231,31 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D53" t="s">
         <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F53" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="G53" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="H53" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I53" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J53" t="s">
         <v>9</v>
       </c>
       <c r="K53" s="2">
-        <v>277171200</v>
+        <v>3880646</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
@@ -5256,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="Q53" s="2">
-        <v>277171200</v>
+        <v>3880646</v>
       </c>
       <c r="R53" s="2">
         <v>0</v>
@@ -5291,37 +5308,37 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D54" t="s">
         <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F54" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="G54" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="H54" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I54" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J54" t="s">
         <v>9</v>
       </c>
       <c r="K54" s="2">
-        <v>27111603</v>
+        <v>277171200</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
       </c>
       <c r="M54" s="2">
-        <v>53879466</v>
+        <v>0</v>
       </c>
       <c r="N54" s="2">
         <v>0</v>
@@ -5333,7 +5350,7 @@
         <v>0</v>
       </c>
       <c r="Q54" s="2">
-        <v>80991069</v>
+        <v>277171200</v>
       </c>
       <c r="R54" s="2">
         <v>0</v>
@@ -5345,7 +5362,7 @@
         <v>0</v>
       </c>
       <c r="U54" s="2">
-        <v>53879466</v>
+        <v>0</v>
       </c>
       <c r="V54" s="2">
         <v>0</v>
@@ -5357,7 +5374,7 @@
         <v>0</v>
       </c>
       <c r="Y54" s="2">
-        <v>53879466</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
@@ -5368,37 +5385,37 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D55" t="s">
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="F55" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="G55" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="H55" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I55" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="J55" t="s">
         <v>9</v>
       </c>
       <c r="K55" s="2">
-        <v>50388480</v>
+        <v>27111603</v>
       </c>
       <c r="L55" s="2">
         <v>0</v>
       </c>
       <c r="M55" s="2">
-        <v>0</v>
+        <v>53879466</v>
       </c>
       <c r="N55" s="2">
         <v>0</v>
@@ -5410,7 +5427,7 @@
         <v>0</v>
       </c>
       <c r="Q55" s="2">
-        <v>50388480</v>
+        <v>80991069</v>
       </c>
       <c r="R55" s="2">
         <v>0</v>
@@ -5422,7 +5439,7 @@
         <v>0</v>
       </c>
       <c r="U55" s="2">
-        <v>0</v>
+        <v>53879466</v>
       </c>
       <c r="V55" s="2">
         <v>0</v>
@@ -5434,7 +5451,7 @@
         <v>0</v>
       </c>
       <c r="Y55" s="2">
-        <v>0</v>
+        <v>53879466</v>
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
@@ -5451,28 +5468,28 @@
         <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G56" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H56" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I56" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J56" t="s">
         <v>9</v>
       </c>
       <c r="K56" s="2">
-        <v>103815691</v>
+        <v>50388480</v>
       </c>
       <c r="L56" s="2">
-        <v>103753094</v>
+        <v>0</v>
       </c>
       <c r="M56" s="2">
         <v>0</v>
@@ -5487,7 +5504,7 @@
         <v>0</v>
       </c>
       <c r="Q56" s="2">
-        <v>207568785</v>
+        <v>50388480</v>
       </c>
       <c r="R56" s="2">
         <v>0</v>
@@ -5522,19 +5539,19 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="F57" t="s">
-        <v>154</v>
+        <v>49</v>
       </c>
       <c r="G57" t="s">
-        <v>155</v>
+        <v>50</v>
       </c>
       <c r="H57" t="s">
         <v>156</v>
@@ -5546,10 +5563,10 @@
         <v>9</v>
       </c>
       <c r="K57" s="2">
-        <v>0</v>
+        <v>103815691</v>
       </c>
       <c r="L57" s="2">
-        <v>0</v>
+        <v>103753094</v>
       </c>
       <c r="M57" s="2">
         <v>0</v>
@@ -5561,10 +5578,10 @@
         <v>0</v>
       </c>
       <c r="P57" s="2">
-        <v>38518911</v>
+        <v>0</v>
       </c>
       <c r="Q57" s="2">
-        <v>38518911</v>
+        <v>207568785</v>
       </c>
       <c r="R57" s="2">
         <v>0</v>
@@ -5608,16 +5625,16 @@
         <v>101</v>
       </c>
       <c r="F58" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G58" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H58" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I58" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J58" t="s">
         <v>9</v>
@@ -5682,13 +5699,13 @@
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="F59" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="G59" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
       <c r="H59" t="s">
         <v>158</v>
@@ -5703,7 +5720,7 @@
         <v>0</v>
       </c>
       <c r="L59" s="2">
-        <v>869498</v>
+        <v>0</v>
       </c>
       <c r="M59" s="2">
         <v>0</v>
@@ -5715,10 +5732,10 @@
         <v>0</v>
       </c>
       <c r="P59" s="2">
-        <v>0</v>
+        <v>38518911</v>
       </c>
       <c r="Q59" s="2">
-        <v>869498</v>
+        <v>38518911</v>
       </c>
       <c r="R59" s="2">
         <v>0</v>
@@ -5739,10 +5756,10 @@
         <v>0</v>
       </c>
       <c r="X59" s="2">
-        <v>0</v>
+        <v>30000000</v>
       </c>
       <c r="Y59" s="2">
-        <v>0</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
@@ -5753,25 +5770,25 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="F60" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="G60" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="H60" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I60" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J60" t="s">
         <v>9</v>
@@ -5780,7 +5797,7 @@
         <v>0</v>
       </c>
       <c r="L60" s="2">
-        <v>150120</v>
+        <v>869498</v>
       </c>
       <c r="M60" s="2">
         <v>0</v>
@@ -5795,7 +5812,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="2">
-        <v>150120</v>
+        <v>869498</v>
       </c>
       <c r="R60" s="2">
         <v>0</v>
@@ -5839,25 +5856,25 @@
         <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="G61" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H61" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="I61" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="J61" t="s">
         <v>9</v>
       </c>
       <c r="K61" s="2">
-        <v>394925760</v>
+        <v>0</v>
       </c>
       <c r="L61" s="2">
-        <v>95283648</v>
+        <v>150120</v>
       </c>
       <c r="M61" s="2">
         <v>0</v>
@@ -5872,7 +5889,7 @@
         <v>0</v>
       </c>
       <c r="Q61" s="2">
-        <v>490209408</v>
+        <v>150120</v>
       </c>
       <c r="R61" s="2">
         <v>0</v>
@@ -5907,34 +5924,34 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
         <v>3</v>
       </c>
       <c r="E62" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F62" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="G62" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="H62" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I62" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J62" t="s">
         <v>9</v>
       </c>
       <c r="K62" s="2">
-        <v>15087916</v>
+        <v>394925760</v>
       </c>
       <c r="L62" s="2">
-        <v>14786158</v>
+        <v>95283648</v>
       </c>
       <c r="M62" s="2">
         <v>0</v>
@@ -5949,7 +5966,7 @@
         <v>0</v>
       </c>
       <c r="Q62" s="2">
-        <v>29874074</v>
+        <v>490209408</v>
       </c>
       <c r="R62" s="2">
         <v>0</v>
@@ -5984,34 +6001,34 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D63" t="s">
         <v>3</v>
       </c>
       <c r="E63" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F63" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="G63" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="H63" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I63" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J63" t="s">
         <v>9</v>
       </c>
       <c r="K63" s="2">
-        <v>354240</v>
+        <v>15087916</v>
       </c>
       <c r="L63" s="2">
-        <v>0</v>
+        <v>14786158</v>
       </c>
       <c r="M63" s="2">
         <v>0</v>
@@ -6026,7 +6043,7 @@
         <v>0</v>
       </c>
       <c r="Q63" s="2">
-        <v>354240</v>
+        <v>29874074</v>
       </c>
       <c r="R63" s="2">
         <v>0</v>
@@ -6070,22 +6087,22 @@
         <v>4</v>
       </c>
       <c r="F64" t="s">
-        <v>15</v>
+        <v>164</v>
       </c>
       <c r="G64" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I64" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="J64" t="s">
         <v>9</v>
       </c>
       <c r="K64" s="2">
-        <v>86512752</v>
+        <v>354240</v>
       </c>
       <c r="L64" s="2">
         <v>0</v>
@@ -6103,7 +6120,7 @@
         <v>0</v>
       </c>
       <c r="Q64" s="2">
-        <v>86512752</v>
+        <v>354240</v>
       </c>
       <c r="R64" s="2">
         <v>0</v>
@@ -6147,25 +6164,25 @@
         <v>4</v>
       </c>
       <c r="F65" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G65" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H65" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I65" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="J65" t="s">
         <v>9</v>
       </c>
       <c r="K65" s="2">
-        <v>245569000</v>
+        <v>86512752</v>
       </c>
       <c r="L65" s="2">
-        <v>214508200</v>
+        <v>0</v>
       </c>
       <c r="M65" s="2">
         <v>0</v>
@@ -6180,7 +6197,7 @@
         <v>0</v>
       </c>
       <c r="Q65" s="2">
-        <v>460077200</v>
+        <v>86512752</v>
       </c>
       <c r="R65" s="2">
         <v>0</v>
@@ -6224,10 +6241,10 @@
         <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="G66" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="H66" t="s">
         <v>171</v>
@@ -6239,10 +6256,10 @@
         <v>9</v>
       </c>
       <c r="K66" s="2">
-        <v>35977392</v>
+        <v>245569000</v>
       </c>
       <c r="L66" s="2">
-        <v>45515952</v>
+        <v>214508200</v>
       </c>
       <c r="M66" s="2">
         <v>0</v>
@@ -6257,7 +6274,7 @@
         <v>0</v>
       </c>
       <c r="Q66" s="2">
-        <v>81493344</v>
+        <v>460077200</v>
       </c>
       <c r="R66" s="2">
         <v>0</v>
@@ -6301,25 +6318,25 @@
         <v>4</v>
       </c>
       <c r="F67" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="G67" t="s">
-        <v>50</v>
+        <v>174</v>
       </c>
       <c r="H67" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I67" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="J67" t="s">
         <v>9</v>
       </c>
       <c r="K67" s="2">
-        <v>708209568</v>
+        <v>35977392</v>
       </c>
       <c r="L67" s="2">
-        <v>0</v>
+        <v>45515952</v>
       </c>
       <c r="M67" s="2">
         <v>0</v>
@@ -6334,7 +6351,7 @@
         <v>0</v>
       </c>
       <c r="Q67" s="2">
-        <v>708209568</v>
+        <v>81493344</v>
       </c>
       <c r="R67" s="2">
         <v>0</v>
@@ -6369,34 +6386,34 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D68" t="s">
         <v>3</v>
       </c>
       <c r="E68" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="F68" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="G68" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="H68" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I68" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="J68" t="s">
         <v>9</v>
       </c>
       <c r="K68" s="2">
-        <v>10235715</v>
+        <v>708209568</v>
       </c>
       <c r="L68" s="2">
-        <v>8519043</v>
+        <v>0</v>
       </c>
       <c r="M68" s="2">
         <v>0</v>
@@ -6405,19 +6422,19 @@
         <v>0</v>
       </c>
       <c r="O68" s="2">
-        <v>44470499</v>
+        <v>0</v>
       </c>
       <c r="P68" s="2">
         <v>0</v>
       </c>
       <c r="Q68" s="2">
-        <v>63225257</v>
+        <v>708209568</v>
       </c>
       <c r="R68" s="2">
         <v>0</v>
       </c>
       <c r="S68" s="2">
-        <v>0</v>
+        <v>102118320</v>
       </c>
       <c r="T68" s="2">
         <v>0</v>
@@ -6435,7 +6452,7 @@
         <v>0</v>
       </c>
       <c r="Y68" s="2">
-        <v>0</v>
+        <v>102118320</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
@@ -6455,25 +6472,25 @@
         <v>101</v>
       </c>
       <c r="F69" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="G69" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="H69" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I69" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J69" t="s">
         <v>9</v>
       </c>
       <c r="K69" s="2">
-        <v>20741602</v>
+        <v>10235715</v>
       </c>
       <c r="L69" s="2">
-        <v>0</v>
+        <v>8519043</v>
       </c>
       <c r="M69" s="2">
         <v>0</v>
@@ -6482,19 +6499,19 @@
         <v>0</v>
       </c>
       <c r="O69" s="2">
-        <v>0</v>
+        <v>44470499</v>
       </c>
       <c r="P69" s="2">
         <v>0</v>
       </c>
       <c r="Q69" s="2">
-        <v>20741602</v>
+        <v>63225257</v>
       </c>
       <c r="R69" s="2">
         <v>0</v>
       </c>
       <c r="S69" s="2">
-        <v>3731522</v>
+        <v>0</v>
       </c>
       <c r="T69" s="2">
         <v>0</v>
@@ -6506,13 +6523,13 @@
         <v>0</v>
       </c>
       <c r="W69" s="2">
-        <v>0</v>
+        <v>15000000</v>
       </c>
       <c r="X69" s="2">
         <v>0</v>
       </c>
       <c r="Y69" s="2">
-        <v>3731522</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
@@ -6523,37 +6540,37 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D70" t="s">
         <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="F70" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="G70" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="H70" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I70" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J70" t="s">
         <v>9</v>
       </c>
       <c r="K70" s="2">
-        <v>0</v>
+        <v>20741602</v>
       </c>
       <c r="L70" s="2">
         <v>0</v>
       </c>
       <c r="M70" s="2">
-        <v>6301584</v>
+        <v>0</v>
       </c>
       <c r="N70" s="2">
         <v>0</v>
@@ -6565,19 +6582,19 @@
         <v>0</v>
       </c>
       <c r="Q70" s="2">
-        <v>6301584</v>
+        <v>20741602</v>
       </c>
       <c r="R70" s="2">
         <v>0</v>
       </c>
       <c r="S70" s="2">
-        <v>0</v>
+        <v>3731522</v>
       </c>
       <c r="T70" s="2">
         <v>0</v>
       </c>
       <c r="U70" s="2">
-        <v>6301584</v>
+        <v>0</v>
       </c>
       <c r="V70" s="2">
         <v>0</v>
@@ -6589,7 +6606,7 @@
         <v>0</v>
       </c>
       <c r="Y70" s="2">
-        <v>6301584</v>
+        <v>3731522</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
@@ -6600,19 +6617,19 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
         <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F71" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>182</v>
+        <v>16</v>
       </c>
       <c r="H71" t="s">
         <v>183</v>
@@ -6624,13 +6641,13 @@
         <v>9</v>
       </c>
       <c r="K71" s="2">
-        <v>5581440</v>
+        <v>0</v>
       </c>
       <c r="L71" s="2">
         <v>0</v>
       </c>
       <c r="M71" s="2">
-        <v>0</v>
+        <v>6301584</v>
       </c>
       <c r="N71" s="2">
         <v>0</v>
@@ -6642,7 +6659,7 @@
         <v>0</v>
       </c>
       <c r="Q71" s="2">
-        <v>5581440</v>
+        <v>6301584</v>
       </c>
       <c r="R71" s="2">
         <v>0</v>
@@ -6654,7 +6671,7 @@
         <v>0</v>
       </c>
       <c r="U71" s="2">
-        <v>0</v>
+        <v>6301584</v>
       </c>
       <c r="V71" s="2">
         <v>0</v>
@@ -6666,7 +6683,7 @@
         <v>0</v>
       </c>
       <c r="Y71" s="2">
-        <v>0</v>
+        <v>6301584</v>
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
@@ -6683,13 +6700,13 @@
         <v>3</v>
       </c>
       <c r="E72" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="F72" t="s">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="G72" t="s">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="H72" t="s">
         <v>185</v>
@@ -6701,10 +6718,10 @@
         <v>9</v>
       </c>
       <c r="K72" s="2">
-        <v>8293106</v>
+        <v>5581440</v>
       </c>
       <c r="L72" s="2">
-        <v>8973326</v>
+        <v>0</v>
       </c>
       <c r="M72" s="2">
         <v>0</v>
@@ -6719,7 +6736,7 @@
         <v>0</v>
       </c>
       <c r="Q72" s="2">
-        <v>17266432</v>
+        <v>5581440</v>
       </c>
       <c r="R72" s="2">
         <v>0</v>
@@ -6760,7 +6777,7 @@
         <v>3</v>
       </c>
       <c r="E73" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="F73" t="s">
         <v>125</v>
@@ -6778,13 +6795,13 @@
         <v>9</v>
       </c>
       <c r="K73" s="2">
-        <v>0</v>
+        <v>8293106</v>
       </c>
       <c r="L73" s="2">
-        <v>0</v>
+        <v>8973326</v>
       </c>
       <c r="M73" s="2">
-        <v>15582617</v>
+        <v>0</v>
       </c>
       <c r="N73" s="2">
         <v>0</v>
@@ -6793,10 +6810,10 @@
         <v>0</v>
       </c>
       <c r="P73" s="2">
-        <v>6181387</v>
+        <v>0</v>
       </c>
       <c r="Q73" s="2">
-        <v>21764004</v>
+        <v>17266432</v>
       </c>
       <c r="R73" s="2">
         <v>0</v>
@@ -6831,19 +6848,19 @@
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D74" t="s">
         <v>3</v>
       </c>
       <c r="E74" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="G74" t="s">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="H74" t="s">
         <v>189</v>
@@ -6855,13 +6872,13 @@
         <v>9</v>
       </c>
       <c r="K74" s="2">
-        <v>227578032</v>
+        <v>0</v>
       </c>
       <c r="L74" s="2">
-        <v>43138224</v>
+        <v>0</v>
       </c>
       <c r="M74" s="2">
-        <v>0</v>
+        <v>15582617</v>
       </c>
       <c r="N74" s="2">
         <v>0</v>
@@ -6870,10 +6887,10 @@
         <v>0</v>
       </c>
       <c r="P74" s="2">
-        <v>0</v>
+        <v>6181387</v>
       </c>
       <c r="Q74" s="2">
-        <v>270716256</v>
+        <v>21764004</v>
       </c>
       <c r="R74" s="2">
         <v>0</v>
@@ -6908,19 +6925,19 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
         <v>3</v>
       </c>
       <c r="E75" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F75" t="s">
-        <v>181</v>
+        <v>10</v>
       </c>
       <c r="G75" t="s">
-        <v>182</v>
+        <v>11</v>
       </c>
       <c r="H75" t="s">
         <v>191</v>
@@ -6932,13 +6949,13 @@
         <v>9</v>
       </c>
       <c r="K75" s="2">
-        <v>45331549</v>
+        <v>227578032</v>
       </c>
       <c r="L75" s="2">
-        <v>0</v>
+        <v>43138224</v>
       </c>
       <c r="M75" s="2">
-        <v>62387128</v>
+        <v>0</v>
       </c>
       <c r="N75" s="2">
         <v>0</v>
@@ -6950,7 +6967,7 @@
         <v>0</v>
       </c>
       <c r="Q75" s="2">
-        <v>107718677</v>
+        <v>270716256</v>
       </c>
       <c r="R75" s="2">
         <v>0</v>
@@ -6985,19 +7002,19 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
         <v>3</v>
       </c>
       <c r="E76" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="G76" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="H76" t="s">
         <v>193</v>
@@ -7009,7 +7026,7 @@
         <v>9</v>
       </c>
       <c r="K76" s="2">
-        <v>92646274</v>
+        <v>89640000</v>
       </c>
       <c r="L76" s="2">
         <v>0</v>
@@ -7027,13 +7044,13 @@
         <v>0</v>
       </c>
       <c r="Q76" s="2">
-        <v>92646274</v>
+        <v>89640000</v>
       </c>
       <c r="R76" s="2">
         <v>0</v>
       </c>
       <c r="S76" s="2">
-        <v>0</v>
+        <v>24900000</v>
       </c>
       <c r="T76" s="2">
         <v>0</v>
@@ -7051,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="Y76" s="2">
-        <v>0</v>
+        <v>24900000</v>
       </c>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
@@ -7062,37 +7079,37 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D77" t="s">
         <v>3</v>
       </c>
       <c r="E77" t="s">
+        <v>96</v>
+      </c>
+      <c r="F77" t="s">
+        <v>125</v>
+      </c>
+      <c r="G77" t="s">
+        <v>126</v>
+      </c>
+      <c r="H77" t="s">
         <v>195</v>
       </c>
-      <c r="F77" t="s">
-        <v>43</v>
-      </c>
-      <c r="G77" t="s">
-        <v>44</v>
-      </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>196</v>
       </c>
-      <c r="I77" t="s">
-        <v>197</v>
-      </c>
       <c r="J77" t="s">
         <v>9</v>
       </c>
       <c r="K77" s="2">
-        <v>75600000</v>
+        <v>45331549</v>
       </c>
       <c r="L77" s="2">
         <v>0</v>
       </c>
       <c r="M77" s="2">
-        <v>0</v>
+        <v>62387128</v>
       </c>
       <c r="N77" s="2">
         <v>0</v>
@@ -7104,7 +7121,7 @@
         <v>0</v>
       </c>
       <c r="Q77" s="2">
-        <v>75600000</v>
+        <v>107718677</v>
       </c>
       <c r="R77" s="2">
         <v>0</v>
@@ -7145,28 +7162,28 @@
         <v>3</v>
       </c>
       <c r="E78" t="s">
+        <v>96</v>
+      </c>
+      <c r="F78" t="s">
+        <v>106</v>
+      </c>
+      <c r="G78" t="s">
+        <v>107</v>
+      </c>
+      <c r="H78" t="s">
+        <v>197</v>
+      </c>
+      <c r="I78" t="s">
         <v>198</v>
       </c>
-      <c r="F78" t="s">
-        <v>125</v>
-      </c>
-      <c r="G78" t="s">
-        <v>126</v>
-      </c>
-      <c r="H78" t="s">
-        <v>199</v>
-      </c>
-      <c r="I78" t="s">
-        <v>200</v>
-      </c>
       <c r="J78" t="s">
         <v>9</v>
       </c>
       <c r="K78" s="2">
-        <v>1446702</v>
+        <v>92646274</v>
       </c>
       <c r="L78" s="2">
-        <v>24638</v>
+        <v>0</v>
       </c>
       <c r="M78" s="2">
         <v>0</v>
@@ -7181,13 +7198,13 @@
         <v>0</v>
       </c>
       <c r="Q78" s="2">
-        <v>1471340</v>
+        <v>92646274</v>
       </c>
       <c r="R78" s="2">
-        <v>71362</v>
+        <v>0</v>
       </c>
       <c r="S78" s="2">
-        <v>641543</v>
+        <v>0</v>
       </c>
       <c r="T78" s="2">
         <v>0</v>
@@ -7205,7 +7222,7 @@
         <v>0</v>
       </c>
       <c r="Y78" s="2">
-        <v>712905</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.25">
@@ -7216,31 +7233,31 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
         <v>3</v>
       </c>
       <c r="E79" t="s">
-        <v>96</v>
+        <v>199</v>
       </c>
       <c r="F79" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="G79" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="H79" t="s">
+        <v>200</v>
+      </c>
+      <c r="I79" t="s">
         <v>201</v>
       </c>
-      <c r="I79" t="s">
-        <v>202</v>
-      </c>
       <c r="J79" t="s">
         <v>9</v>
       </c>
       <c r="K79" s="2">
-        <v>11840521</v>
+        <v>75600000</v>
       </c>
       <c r="L79" s="2">
         <v>0</v>
@@ -7258,7 +7275,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="2">
-        <v>11840521</v>
+        <v>75600000</v>
       </c>
       <c r="R79" s="2">
         <v>0</v>
@@ -7299,13 +7316,13 @@
         <v>3</v>
       </c>
       <c r="E80" t="s">
-        <v>96</v>
+        <v>202</v>
       </c>
       <c r="F80" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="G80" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="H80" t="s">
         <v>203</v>
@@ -7317,10 +7334,10 @@
         <v>9</v>
       </c>
       <c r="K80" s="2">
-        <v>6514266</v>
+        <v>1446702</v>
       </c>
       <c r="L80" s="2">
-        <v>0</v>
+        <v>24638</v>
       </c>
       <c r="M80" s="2">
         <v>0</v>
@@ -7335,13 +7352,13 @@
         <v>0</v>
       </c>
       <c r="Q80" s="2">
-        <v>6514266</v>
+        <v>1471340</v>
       </c>
       <c r="R80" s="2">
-        <v>0</v>
+        <v>71362</v>
       </c>
       <c r="S80" s="2">
-        <v>0</v>
+        <v>641543</v>
       </c>
       <c r="T80" s="2">
         <v>0</v>
@@ -7359,7 +7376,7 @@
         <v>0</v>
       </c>
       <c r="Y80" s="2">
-        <v>0</v>
+        <v>712905</v>
       </c>
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
@@ -7370,19 +7387,19 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D81" t="s">
         <v>3</v>
       </c>
       <c r="E81" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F81" t="s">
-        <v>160</v>
+        <v>106</v>
       </c>
       <c r="G81" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="H81" t="s">
         <v>205</v>
@@ -7394,10 +7411,10 @@
         <v>9</v>
       </c>
       <c r="K81" s="2">
-        <v>0</v>
+        <v>11840521</v>
       </c>
       <c r="L81" s="2">
-        <v>1287576</v>
+        <v>0</v>
       </c>
       <c r="M81" s="2">
         <v>0</v>
@@ -7412,7 +7429,7 @@
         <v>0</v>
       </c>
       <c r="Q81" s="2">
-        <v>1287576</v>
+        <v>11840521</v>
       </c>
       <c r="R81" s="2">
         <v>0</v>
@@ -7447,34 +7464,34 @@
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D82" t="s">
         <v>3</v>
       </c>
       <c r="E82" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F82" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="G82" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="H82" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="I82" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J82" t="s">
         <v>9</v>
       </c>
       <c r="K82" s="2">
-        <v>0</v>
+        <v>6514266</v>
       </c>
       <c r="L82" s="2">
-        <v>8756640</v>
+        <v>0</v>
       </c>
       <c r="M82" s="2">
         <v>0</v>
@@ -7489,7 +7506,7 @@
         <v>0</v>
       </c>
       <c r="Q82" s="2">
-        <v>8756640</v>
+        <v>6514266</v>
       </c>
       <c r="R82" s="2">
         <v>0</v>
@@ -7524,34 +7541,34 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
         <v>3</v>
       </c>
       <c r="E83" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>110</v>
+        <v>164</v>
       </c>
       <c r="G83" t="s">
-        <v>111</v>
+        <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I83" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J83" t="s">
         <v>9</v>
       </c>
       <c r="K83" s="2">
-        <v>6293384</v>
+        <v>0</v>
       </c>
       <c r="L83" s="2">
-        <v>0</v>
+        <v>1287576</v>
       </c>
       <c r="M83" s="2">
         <v>0</v>
@@ -7566,7 +7583,7 @@
         <v>0</v>
       </c>
       <c r="Q83" s="2">
-        <v>6293384</v>
+        <v>1287576</v>
       </c>
       <c r="R83" s="2">
         <v>0</v>
@@ -7610,10 +7627,10 @@
         <v>4</v>
       </c>
       <c r="F84" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H84" t="s">
         <v>209</v>
@@ -7625,10 +7642,10 @@
         <v>9</v>
       </c>
       <c r="K84" s="2">
-        <v>4968000</v>
+        <v>0</v>
       </c>
       <c r="L84" s="2">
-        <v>0</v>
+        <v>8756640</v>
       </c>
       <c r="M84" s="2">
         <v>0</v>
@@ -7643,7 +7660,7 @@
         <v>0</v>
       </c>
       <c r="Q84" s="2">
-        <v>4968000</v>
+        <v>8756640</v>
       </c>
       <c r="R84" s="2">
         <v>0</v>
@@ -7687,10 +7704,10 @@
         <v>96</v>
       </c>
       <c r="F85" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="G85" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="H85" t="s">
         <v>211</v>
@@ -7702,10 +7719,10 @@
         <v>9</v>
       </c>
       <c r="K85" s="2">
-        <v>15552000</v>
+        <v>6293384</v>
       </c>
       <c r="L85" s="2">
-        <v>31735068</v>
+        <v>0</v>
       </c>
       <c r="M85" s="2">
         <v>0</v>
@@ -7720,7 +7737,7 @@
         <v>0</v>
       </c>
       <c r="Q85" s="2">
-        <v>47287068</v>
+        <v>6293384</v>
       </c>
       <c r="R85" s="2">
         <v>0</v>
@@ -7755,19 +7772,19 @@
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
         <v>3</v>
       </c>
       <c r="E86" t="s">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="F86" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="G86" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="H86" t="s">
         <v>213</v>
@@ -7779,7 +7796,7 @@
         <v>9</v>
       </c>
       <c r="K86" s="2">
-        <v>43365268</v>
+        <v>4968000</v>
       </c>
       <c r="L86" s="2">
         <v>0</v>
@@ -7797,13 +7814,13 @@
         <v>0</v>
       </c>
       <c r="Q86" s="2">
-        <v>43365268</v>
+        <v>4968000</v>
       </c>
       <c r="R86" s="2">
         <v>0</v>
       </c>
       <c r="S86" s="2">
-        <v>21382589</v>
+        <v>0</v>
       </c>
       <c r="T86" s="2">
         <v>0</v>
@@ -7821,7 +7838,7 @@
         <v>0</v>
       </c>
       <c r="Y86" s="2">
-        <v>21382589</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.25">
@@ -7832,34 +7849,34 @@
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D87" t="s">
         <v>3</v>
       </c>
       <c r="E87" t="s">
+        <v>96</v>
+      </c>
+      <c r="F87" t="s">
+        <v>129</v>
+      </c>
+      <c r="G87" t="s">
+        <v>130</v>
+      </c>
+      <c r="H87" t="s">
         <v>215</v>
       </c>
-      <c r="F87" t="s">
-        <v>79</v>
-      </c>
-      <c r="G87" t="s">
-        <v>80</v>
-      </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>216</v>
       </c>
-      <c r="I87" t="s">
-        <v>217</v>
-      </c>
       <c r="J87" t="s">
         <v>9</v>
       </c>
       <c r="K87" s="2">
-        <v>520636036</v>
+        <v>15552000</v>
       </c>
       <c r="L87" s="2">
-        <v>0</v>
+        <v>31735068</v>
       </c>
       <c r="M87" s="2">
         <v>0</v>
@@ -7874,7 +7891,7 @@
         <v>0</v>
       </c>
       <c r="Q87" s="2">
-        <v>520636036</v>
+        <v>47287068</v>
       </c>
       <c r="R87" s="2">
         <v>0</v>
@@ -7909,19 +7926,19 @@
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
         <v>3</v>
       </c>
       <c r="E88" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
       <c r="F88" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="G88" t="s">
-        <v>182</v>
+        <v>80</v>
       </c>
       <c r="H88" t="s">
         <v>218</v>
@@ -7933,7 +7950,7 @@
         <v>9</v>
       </c>
       <c r="K88" s="2">
-        <v>0</v>
+        <v>520636036</v>
       </c>
       <c r="L88" s="2">
         <v>0</v>
@@ -7945,13 +7962,13 @@
         <v>0</v>
       </c>
       <c r="O88" s="2">
-        <v>-437763</v>
+        <v>0</v>
       </c>
       <c r="P88" s="2">
-        <v>-563094</v>
+        <v>0</v>
       </c>
       <c r="Q88" s="2">
-        <v>-1000857</v>
+        <v>520636036</v>
       </c>
       <c r="R88" s="2">
         <v>0</v>
@@ -7995,10 +8012,10 @@
         <v>101</v>
       </c>
       <c r="F89" t="s">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="G89" t="s">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="H89" t="s">
         <v>220</v>
@@ -8072,10 +8089,10 @@
         <v>101</v>
       </c>
       <c r="F90" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G90" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H90" t="s">
         <v>222</v>
@@ -8149,10 +8166,10 @@
         <v>96</v>
       </c>
       <c r="F91" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G91" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H91" t="s">
         <v>224</v>
@@ -8226,10 +8243,10 @@
         <v>96</v>
       </c>
       <c r="F92" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="G92" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H92" t="s">
         <v>226</v>
@@ -8371,19 +8388,19 @@
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="D94" t="s">
         <v>3</v>
       </c>
       <c r="E94" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="F94" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="G94" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="H94" t="s">
         <v>230</v>
@@ -8395,7 +8412,7 @@
         <v>9</v>
       </c>
       <c r="K94" s="2">
-        <v>13588560</v>
+        <v>55983640</v>
       </c>
       <c r="L94" s="2">
         <v>0</v>
@@ -8413,13 +8430,13 @@
         <v>0</v>
       </c>
       <c r="Q94" s="2">
-        <v>13588560</v>
+        <v>55983640</v>
       </c>
       <c r="R94" s="2">
         <v>0</v>
       </c>
       <c r="S94" s="2">
-        <v>13588560</v>
+        <v>56402906</v>
       </c>
       <c r="T94" s="2">
         <v>0</v>
@@ -8437,7 +8454,7 @@
         <v>0</v>
       </c>
       <c r="Y94" s="2">
-        <v>13588560</v>
+        <v>56402906</v>
       </c>
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
@@ -8457,10 +8474,10 @@
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="G95" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="H95" t="s">
         <v>232</v>
@@ -8472,7 +8489,7 @@
         <v>9</v>
       </c>
       <c r="K95" s="2">
-        <v>8359200</v>
+        <v>13588560</v>
       </c>
       <c r="L95" s="2">
         <v>0</v>
@@ -8490,13 +8507,13 @@
         <v>0</v>
       </c>
       <c r="Q95" s="2">
-        <v>8359200</v>
+        <v>13588560</v>
       </c>
       <c r="R95" s="2">
         <v>0</v>
       </c>
       <c r="S95" s="2">
-        <v>8359200</v>
+        <v>13588560</v>
       </c>
       <c r="T95" s="2">
         <v>0</v>
@@ -8514,7 +8531,7 @@
         <v>0</v>
       </c>
       <c r="Y95" s="2">
-        <v>8359200</v>
+        <v>13588560</v>
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
@@ -8534,10 +8551,10 @@
         <v>4</v>
       </c>
       <c r="F96" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G96" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H96" t="s">
         <v>234</v>
@@ -8549,7 +8566,7 @@
         <v>9</v>
       </c>
       <c r="K96" s="2">
-        <v>1935360</v>
+        <v>8359200</v>
       </c>
       <c r="L96" s="2">
         <v>0</v>
@@ -8567,13 +8584,13 @@
         <v>0</v>
       </c>
       <c r="Q96" s="2">
-        <v>1935360</v>
+        <v>8359200</v>
       </c>
       <c r="R96" s="2">
         <v>0</v>
       </c>
       <c r="S96" s="2">
-        <v>1935360</v>
+        <v>8359200</v>
       </c>
       <c r="T96" s="2">
         <v>0</v>
@@ -8591,7 +8608,7 @@
         <v>0</v>
       </c>
       <c r="Y96" s="2">
-        <v>1935360</v>
+        <v>8359200</v>
       </c>
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
@@ -8602,19 +8619,19 @@
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>3</v>
       </c>
       <c r="E97" t="s">
-        <v>198</v>
+        <v>4</v>
       </c>
       <c r="F97" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="G97" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="H97" t="s">
         <v>236</v>
@@ -8626,7 +8643,7 @@
         <v>9</v>
       </c>
       <c r="K97" s="2">
-        <v>7318080</v>
+        <v>1935360</v>
       </c>
       <c r="L97" s="2">
         <v>0</v>
@@ -8644,13 +8661,13 @@
         <v>0</v>
       </c>
       <c r="Q97" s="2">
-        <v>7318080</v>
+        <v>1935360</v>
       </c>
       <c r="R97" s="2">
         <v>0</v>
       </c>
       <c r="S97" s="2">
-        <v>7318080</v>
+        <v>1935360</v>
       </c>
       <c r="T97" s="2">
         <v>0</v>
@@ -8668,7 +8685,7 @@
         <v>0</v>
       </c>
       <c r="Y97" s="2">
-        <v>7318080</v>
+        <v>1935360</v>
       </c>
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
@@ -8679,19 +8696,19 @@
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D98" t="s">
         <v>3</v>
       </c>
       <c r="E98" t="s">
-        <v>118</v>
+        <v>202</v>
       </c>
       <c r="F98" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
       <c r="G98" t="s">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="H98" t="s">
         <v>238</v>
@@ -8703,7 +8720,7 @@
         <v>9</v>
       </c>
       <c r="K98" s="2">
-        <v>4814059</v>
+        <v>7318080</v>
       </c>
       <c r="L98" s="2">
         <v>0</v>
@@ -8721,13 +8738,13 @@
         <v>0</v>
       </c>
       <c r="Q98" s="2">
-        <v>4814059</v>
+        <v>7318080</v>
       </c>
       <c r="R98" s="2">
         <v>0</v>
       </c>
       <c r="S98" s="2">
-        <v>4814059</v>
+        <v>7318080</v>
       </c>
       <c r="T98" s="2">
         <v>0</v>
@@ -8745,7 +8762,7 @@
         <v>0</v>
       </c>
       <c r="Y98" s="2">
-        <v>4814059</v>
+        <v>7318080</v>
       </c>
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.25">
@@ -8756,19 +8773,19 @@
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="D99" t="s">
         <v>3</v>
       </c>
       <c r="E99" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="F99" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="G99" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="H99" t="s">
         <v>240</v>
@@ -8780,53 +8797,284 @@
         <v>9</v>
       </c>
       <c r="K99" s="2">
+        <v>4814059</v>
+      </c>
+      <c r="L99" s="2">
+        <v>0</v>
+      </c>
+      <c r="M99" s="2">
+        <v>0</v>
+      </c>
+      <c r="N99" s="2">
+        <v>0</v>
+      </c>
+      <c r="O99" s="2">
+        <v>0</v>
+      </c>
+      <c r="P99" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="2">
+        <v>4814059</v>
+      </c>
+      <c r="R99" s="2">
+        <v>0</v>
+      </c>
+      <c r="S99" s="2">
+        <v>4814059</v>
+      </c>
+      <c r="T99" s="2">
+        <v>0</v>
+      </c>
+      <c r="U99" s="2">
+        <v>0</v>
+      </c>
+      <c r="V99" s="2">
+        <v>0</v>
+      </c>
+      <c r="W99" s="2">
+        <v>0</v>
+      </c>
+      <c r="X99" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y99" s="2">
+        <v>4814059</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>65</v>
+      </c>
+      <c r="D100" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100" t="s">
+        <v>141</v>
+      </c>
+      <c r="F100" t="s">
+        <v>71</v>
+      </c>
+      <c r="G100" t="s">
+        <v>72</v>
+      </c>
+      <c r="H100" t="s">
+        <v>242</v>
+      </c>
+      <c r="I100" t="s">
+        <v>243</v>
+      </c>
+      <c r="J100" t="s">
+        <v>9</v>
+      </c>
+      <c r="K100" s="2">
         <v>10200000</v>
       </c>
-      <c r="L99" s="2">
-        <v>0</v>
-      </c>
-      <c r="M99" s="2">
-        <v>0</v>
-      </c>
-      <c r="N99" s="2">
-        <v>0</v>
-      </c>
-      <c r="O99" s="2">
-        <v>0</v>
-      </c>
-      <c r="P99" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="2">
+      <c r="L100" s="2">
+        <v>0</v>
+      </c>
+      <c r="M100" s="2">
+        <v>0</v>
+      </c>
+      <c r="N100" s="2">
+        <v>0</v>
+      </c>
+      <c r="O100" s="2">
+        <v>0</v>
+      </c>
+      <c r="P100" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="2">
         <v>10200000</v>
       </c>
-      <c r="R99" s="2">
-        <v>0</v>
-      </c>
-      <c r="S99" s="2">
+      <c r="R100" s="2">
+        <v>0</v>
+      </c>
+      <c r="S100" s="2">
         <v>10200000</v>
       </c>
-      <c r="T99" s="2">
-        <v>0</v>
-      </c>
-      <c r="U99" s="2">
-        <v>0</v>
-      </c>
-      <c r="V99" s="2">
-        <v>0</v>
-      </c>
-      <c r="W99" s="2">
-        <v>0</v>
-      </c>
-      <c r="X99" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y99" s="2">
+      <c r="T100" s="2">
+        <v>0</v>
+      </c>
+      <c r="U100" s="2">
+        <v>0</v>
+      </c>
+      <c r="V100" s="2">
+        <v>0</v>
+      </c>
+      <c r="W100" s="2">
+        <v>0</v>
+      </c>
+      <c r="X100" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y100" s="2">
         <v>10200000</v>
       </c>
     </row>
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" t="s">
+        <v>173</v>
+      </c>
+      <c r="G101" t="s">
+        <v>174</v>
+      </c>
+      <c r="H101" t="s">
+        <v>244</v>
+      </c>
+      <c r="I101" t="s">
+        <v>245</v>
+      </c>
+      <c r="J101" t="s">
+        <v>9</v>
+      </c>
+      <c r="K101" s="2">
+        <v>15970608</v>
+      </c>
+      <c r="L101" s="2">
+        <v>0</v>
+      </c>
+      <c r="M101" s="2">
+        <v>0</v>
+      </c>
+      <c r="N101" s="2">
+        <v>0</v>
+      </c>
+      <c r="O101" s="2">
+        <v>0</v>
+      </c>
+      <c r="P101" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="2">
+        <v>15970608</v>
+      </c>
+      <c r="R101" s="2">
+        <v>0</v>
+      </c>
+      <c r="S101" s="2">
+        <v>15970608</v>
+      </c>
+      <c r="T101" s="2">
+        <v>0</v>
+      </c>
+      <c r="U101" s="2">
+        <v>0</v>
+      </c>
+      <c r="V101" s="2">
+        <v>0</v>
+      </c>
+      <c r="W101" s="2">
+        <v>0</v>
+      </c>
+      <c r="X101" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y101" s="2">
+        <v>15970608</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>3</v>
+      </c>
+      <c r="E102" t="s">
+        <v>4</v>
+      </c>
+      <c r="F102" t="s">
+        <v>5</v>
+      </c>
+      <c r="G102" t="s">
+        <v>6</v>
+      </c>
+      <c r="H102" t="s">
+        <v>246</v>
+      </c>
+      <c r="I102" t="s">
+        <v>247</v>
+      </c>
+      <c r="J102" t="s">
+        <v>9</v>
+      </c>
+      <c r="K102" s="2">
+        <v>3361824</v>
+      </c>
+      <c r="L102" s="2">
+        <v>0</v>
+      </c>
+      <c r="M102" s="2">
+        <v>0</v>
+      </c>
+      <c r="N102" s="2">
+        <v>0</v>
+      </c>
+      <c r="O102" s="2">
+        <v>0</v>
+      </c>
+      <c r="P102" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="2">
+        <v>3361824</v>
+      </c>
+      <c r="R102" s="2">
+        <v>0</v>
+      </c>
+      <c r="S102" s="2">
+        <v>3361824</v>
+      </c>
+      <c r="T102" s="2">
+        <v>0</v>
+      </c>
+      <c r="U102" s="2">
+        <v>0</v>
+      </c>
+      <c r="V102" s="2">
+        <v>0</v>
+      </c>
+      <c r="W102" s="2">
+        <v>0</v>
+      </c>
+      <c r="X102" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y102" s="2">
+        <v>3361824</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Y99"/>
+  <autoFilter ref="A1:Y102"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>